<commit_message>
feat: cyclical cookie clearing & finall
</commit_message>
<xml_diff>
--- a/Evaluation.xlsx
+++ b/Evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOS\MasterScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FAD0DD-CA24-4B98-BCC7-E5F8AFBA2FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3C10FB-A39B-42BF-A77A-33809F890697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="38616" windowHeight="21216" activeTab="5" xr2:uid="{105C7B9D-B024-45E8-A2DF-E9EE949B723F}"/>
   </bookViews>
@@ -8906,14 +8906,9 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CEFB5EC4-670D-4CBA-912C-DDD47EE336DE}" name="data_2" displayName="data_2" ref="A1:Y191" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:Y191" xr:uid="{84FF8E89-A7FE-4A28-834F-73CEF16826B7}">
-    <filterColumn colId="11">
+    <filterColumn colId="2">
       <filters>
-        <dateGroupItem year="2021" month="5" dateTimeGrouping="month"/>
-        <dateGroupItem year="2021" month="6" dateTimeGrouping="month"/>
-        <dateGroupItem year="2021" month="7" dateTimeGrouping="month"/>
-        <dateGroupItem year="2021" month="8" dateTimeGrouping="month"/>
-        <dateGroupItem year="2021" month="9" dateTimeGrouping="month"/>
-        <dateGroupItem year="2021" month="11" dateTimeGrouping="month"/>
+        <filter val="Copenhagen"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -49143,10 +49138,10 @@
   <dimension ref="A1:Y191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W186" sqref="W186"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49394,7 +49389,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -49471,7 +49466,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -49544,7 +49539,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>89</v>
       </c>
@@ -51300,7 +51295,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>158</v>
       </c>
@@ -51367,7 +51362,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>144</v>
       </c>
@@ -51436,7 +51431,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>159</v>
       </c>
@@ -51509,7 +51504,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>128</v>
       </c>
@@ -51578,7 +51573,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>130</v>
       </c>
@@ -51724,7 +51719,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>157</v>
       </c>
@@ -51797,7 +51792,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>166</v>
       </c>
@@ -52228,7 +52223,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>131</v>
       </c>
@@ -52299,7 +52294,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>132</v>
       </c>
@@ -52367,7 +52362,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>65</v>
       </c>
@@ -52512,7 +52507,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>61</v>
       </c>
@@ -52583,7 +52578,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>98</v>
       </c>
@@ -52654,7 +52649,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>169</v>
       </c>
@@ -52725,7 +52720,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>155</v>
       </c>
@@ -53571,7 +53566,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>149</v>
       </c>
@@ -53784,7 +53779,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>150</v>
       </c>
@@ -53857,7 +53852,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>174</v>
       </c>
@@ -53928,7 +53923,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>34</v>
       </c>
@@ -53999,7 +53994,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>49</v>
       </c>
@@ -54076,7 +54071,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>181</v>
       </c>
@@ -54147,7 +54142,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>100</v>
       </c>
@@ -54224,7 +54219,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>183</v>
       </c>
@@ -54295,7 +54290,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>118</v>
       </c>
@@ -54366,7 +54361,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>161</v>
       </c>
@@ -54437,7 +54432,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>185</v>
       </c>
@@ -54508,7 +54503,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:25" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>102</v>
       </c>
@@ -54639,7 +54634,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>106</v>
       </c>
@@ -54710,7 +54705,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>138</v>
       </c>
@@ -54854,7 +54849,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>41</v>
       </c>
@@ -54925,7 +54920,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>31</v>
       </c>
@@ -54996,7 +54991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>125</v>
       </c>
@@ -55067,7 +55062,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>37</v>
       </c>
@@ -55215,7 +55210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>127</v>
       </c>
@@ -55286,7 +55281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>168</v>
       </c>
@@ -55354,7 +55349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -55425,7 +55420,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>66</v>
       </c>
@@ -55638,7 +55633,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>114</v>
       </c>
@@ -55774,7 +55769,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>70</v>
       </c>
@@ -55839,7 +55834,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>146</v>
       </c>
@@ -57052,7 +57047,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>164</v>
       </c>
@@ -57123,7 +57118,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>151</v>
       </c>
@@ -57336,7 +57331,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>123</v>
       </c>
@@ -57401,7 +57396,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>59</v>
       </c>
@@ -57614,7 +57609,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>160</v>
       </c>
@@ -57685,7 +57680,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>82</v>
       </c>
@@ -58243,7 +58238,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>3</v>
       </c>
@@ -58308,7 +58303,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>101</v>
       </c>
@@ -58523,7 +58518,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>111</v>
       </c>
@@ -58730,7 +58725,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>86</v>
       </c>
@@ -58798,7 +58793,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>187</v>
       </c>
@@ -58865,7 +58860,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>189</v>
       </c>
@@ -59011,7 +59006,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>122</v>
       </c>
@@ -59078,7 +59073,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>178</v>
       </c>
@@ -59149,7 +59144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>170</v>
       </c>
@@ -59493,7 +59488,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>129</v>
       </c>
@@ -59560,7 +59555,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>142</v>
       </c>
@@ -59747,7 +59742,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>45</v>
       </c>
@@ -59961,7 +59956,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>30</v>
       </c>
@@ -60028,7 +60023,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>95</v>
       </c>
@@ -60099,7 +60094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>87</v>
       </c>
@@ -60170,7 +60165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>53</v>
       </c>
@@ -60241,7 +60236,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>90</v>
       </c>
@@ -60383,7 +60378,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>54</v>
       </c>
@@ -60523,7 +60518,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>139</v>
       </c>
@@ -60723,7 +60718,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>39</v>
       </c>
@@ -60926,7 +60921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>141</v>
       </c>
@@ -61191,7 +61186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>52</v>
       </c>
@@ -61391,7 +61386,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>57</v>
       </c>
@@ -61584,7 +61579,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>43</v>
       </c>
@@ -61719,7 +61714,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>175</v>
       </c>
@@ -61989,7 +61984,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>186</v>
       </c>
@@ -62180,7 +62175,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>10</v>
       </c>
@@ -62324,7 +62319,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>78</v>
       </c>

</xml_diff>